<commit_message>
updated Closed and Open event cases and multiuser cases
</commit_message>
<xml_diff>
--- a/test-data/Vdata.xlsx
+++ b/test-data/Vdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KumarBSantha-MFCWL\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mfcwl Projects\ediig-test\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE9B38B-42A7-4F81-8972-D2CB0ADDE7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9162D9D6-0AF0-4A54-8AB6-AFAB368AE86C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7136C6DB-F0CC-4C33-9575-655EDF0AB019}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="347">
   <si>
     <t>Contract Number</t>
   </si>
@@ -1077,6 +1077,9 @@
   </si>
   <si>
     <t>FE</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -1559,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9FB8548-1DB1-45D3-907D-98AD729327FF}">
   <dimension ref="A1:AC121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1722,7 @@
       <c r="O2" s="12"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R2" s="8" t="s">
         <v>33</v>
@@ -1779,7 +1782,7 @@
       <c r="O3" s="12"/>
       <c r="P3" s="12"/>
       <c r="Q3" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R3" s="8" t="s">
         <v>36</v>
@@ -1839,7 +1842,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R4" s="8" t="s">
         <v>38</v>
@@ -1899,7 +1902,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>40</v>
@@ -1959,7 +1962,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>42</v>
@@ -2019,7 +2022,7 @@
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>43</v>
@@ -2079,7 +2082,7 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
       <c r="Q8" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R8" s="8" t="s">
         <v>46</v>
@@ -2139,7 +2142,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
       <c r="Q9" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R9" s="8" t="s">
         <v>48</v>
@@ -2199,7 +2202,7 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>50</v>
@@ -2259,7 +2262,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R11" s="8" t="s">
         <v>51</v>
@@ -2319,7 +2322,7 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R12" s="8" t="s">
         <v>53</v>
@@ -2379,7 +2382,7 @@
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R13" s="8" t="s">
         <v>55</v>
@@ -2439,7 +2442,7 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R14" s="8" t="s">
         <v>33</v>
@@ -2499,7 +2502,7 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R15" s="8" t="s">
         <v>36</v>
@@ -2559,7 +2562,7 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R16" s="8" t="s">
         <v>38</v>
@@ -2619,7 +2622,7 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R17" s="8" t="s">
         <v>40</v>
@@ -2679,7 +2682,7 @@
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R18" s="8" t="s">
         <v>42</v>
@@ -2739,7 +2742,7 @@
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
       <c r="Q19" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R19" s="8" t="s">
         <v>43</v>
@@ -2799,7 +2802,7 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
       <c r="Q20" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R20" s="8" t="s">
         <v>46</v>
@@ -2859,7 +2862,7 @@
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R21" s="8" t="s">
         <v>48</v>
@@ -2919,7 +2922,7 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R22" s="8" t="s">
         <v>50</v>
@@ -2979,7 +2982,7 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R23" s="8" t="s">
         <v>51</v>
@@ -3039,7 +3042,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R24" s="8" t="s">
         <v>53</v>
@@ -3099,7 +3102,7 @@
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R25" s="8" t="s">
         <v>57</v>
@@ -3159,7 +3162,7 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R26" s="8" t="s">
         <v>59</v>
@@ -3219,7 +3222,7 @@
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R27" s="8" t="s">
         <v>61</v>
@@ -3279,7 +3282,7 @@
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R28" s="8" t="s">
         <v>63</v>
@@ -3336,7 +3339,7 @@
         <v>32</v>
       </c>
       <c r="Q29" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="R29" s="8" t="s">
         <v>65</v>

</xml_diff>